<commit_message>
Cloud pentru campaings images
</commit_message>
<xml_diff>
--- a/src/api/utils/statistici/infractiuni-2021.xlsx
+++ b/src/api/utils/statistici/infractiuni-2021.xlsx
@@ -1,6 +1,6 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26327"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -8,13 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Facultate\tw 20.06.2023\Proiect-Tw\src\api\utils\statistici\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{207803D7-6084-4599-8AB5-D81C24ADFEA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="10500" windowHeight="15600" xr2:uid="{AC1D400B-93D5-43FE-865E-3CDB32BBCAD2}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="10815" windowHeight="15600" activeTab="0"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="1" r:id="rId3"/>
   </sheets>
+  <definedNames/>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
@@ -81,9 +81,6 @@
     <t>Filtru</t>
   </si>
   <si>
-    <t>Incadrare</t>
-  </si>
-  <si>
     <t>Gen</t>
   </si>
   <si>
@@ -109,13 +106,16 @@
   </si>
   <si>
     <t>Persoane în grupări</t>
+  </si>
+  <si>
+    <t>Incadrare juridica</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -123,6 +123,12 @@
       <family val="2"/>
       <charset val="238"/>
       <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="8"/>
@@ -150,32 +156,125 @@
     </border>
     <border>
       <left style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </right>
       <top style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </top>
       <bottom style="thin">
-        <color indexed="64"/>
+        <color auto="1"/>
       </bottom>
-      <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+  <cellStyleXfs count="20">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0">
+      <alignment/>
+      <protection/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="41" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
   <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="6">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Percent" xfId="15" builtinId="5"/>
+    <cellStyle name="Currency" xfId="16" builtinId="4"/>
+    <cellStyle name="Currency [0]" xfId="17" builtinId="7"/>
+    <cellStyle name="Comma" xfId="18" builtinId="3"/>
+    <cellStyle name="Comma [0]" xfId="19" builtinId="6"/>
   </cellStyles>
-  <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <colors>
+    <indexedColors>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00000000"/>
+      <rgbColor rgb="00FFFFFF"/>
+      <rgbColor rgb="00FF0000"/>
+      <rgbColor rgb="0000FF00"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008000"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00808000"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="00C0C0C0"/>
+      <rgbColor rgb="00808080"/>
+      <rgbColor rgb="009999FF"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00FFFFCC"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00660066"/>
+      <rgbColor rgb="00FF8080"/>
+      <rgbColor rgb="000066CC"/>
+      <rgbColor rgb="00CCCCFF"/>
+      <rgbColor rgb="00000080"/>
+      <rgbColor rgb="00FF00FF"/>
+      <rgbColor rgb="00FFFF00"/>
+      <rgbColor rgb="0000FFFF"/>
+      <rgbColor rgb="00800080"/>
+      <rgbColor rgb="00800000"/>
+      <rgbColor rgb="00008080"/>
+      <rgbColor rgb="000000FF"/>
+      <rgbColor rgb="0000CCFF"/>
+      <rgbColor rgb="00CCFFFF"/>
+      <rgbColor rgb="00CCFFCC"/>
+      <rgbColor rgb="00FFFF99"/>
+      <rgbColor rgb="0099CCFF"/>
+      <rgbColor rgb="00FF99CC"/>
+      <rgbColor rgb="00CC99FF"/>
+      <rgbColor rgb="00FFCC99"/>
+      <rgbColor rgb="003366FF"/>
+      <rgbColor rgb="0033CCCC"/>
+      <rgbColor rgb="0099CC00"/>
+      <rgbColor rgb="00FFCC00"/>
+      <rgbColor rgb="00FF9900"/>
+      <rgbColor rgb="00FF6600"/>
+      <rgbColor rgb="00666699"/>
+      <rgbColor rgb="00969696"/>
+      <rgbColor rgb="00003366"/>
+      <rgbColor rgb="00339966"/>
+      <rgbColor rgb="00003300"/>
+      <rgbColor rgb="00333300"/>
+      <rgbColor rgb="00993300"/>
+      <rgbColor rgb="00993366"/>
+      <rgbColor rgb="00333399"/>
+      <rgbColor rgb="00333333"/>
+    </indexedColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -483,22 +582,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF54E5B-9CD9-4AA6-A123-6BF269B1AB33}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xm="http://schemas.microsoft.com/office/excel/2006/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0FF54E5B-9CD9-4AA6-A123-6BF269B1AB33}">
   <dimension ref="A1:D23"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E4" sqref="E4"/>
+    <sheetView tabSelected="1" workbookViewId="0" topLeftCell="A1">
+      <selection pane="topLeft" activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="10.7109375" customWidth="1"/>
-    <col min="2" max="2" width="10.42578125" customWidth="1"/>
-    <col min="3" max="3" width="25.28515625" customWidth="1"/>
-    <col min="4" max="4" width="17.85546875" customWidth="1"/>
+    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="2" max="2" width="10.428571428571429" customWidth="1"/>
+    <col min="3" max="3" width="25.285714285714285" customWidth="1"/>
+    <col min="4" max="4" width="17.857142857142858" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="15">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -509,237 +608,237 @@
         <v>17</v>
       </c>
       <c r="D1" t="s">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" ht="15">
       <c r="A2" t="s">
         <v>1</v>
       </c>
       <c r="B2">
-        <v>10102</v>
+        <v>9845</v>
       </c>
       <c r="C2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:3" ht="15">
       <c r="A3" t="s">
         <v>1</v>
       </c>
       <c r="B3">
-        <v>2413</v>
+        <v>2013</v>
       </c>
       <c r="C3" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" ht="15">
       <c r="A4" t="s">
         <v>1</v>
       </c>
       <c r="B4">
-        <v>1031</v>
+        <v>876</v>
       </c>
       <c r="C4" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:3" ht="15">
       <c r="A5" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B5" s="1">
-        <v>559</v>
+        <v>432</v>
       </c>
       <c r="C5" s="1" t="s">
         <v>4</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:3" ht="15">
       <c r="A6" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B6" s="1">
-        <v>54</v>
+        <v>87</v>
       </c>
       <c r="C6" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:3" ht="15">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1">
-        <v>354</v>
+        <v>313</v>
       </c>
       <c r="C7" t="s">
         <v>6</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:3" ht="15">
       <c r="A8" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B8" s="1">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="C8" t="s">
         <v>7</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:3" ht="15">
       <c r="A9" t="s">
-        <v>18</v>
+        <v>27</v>
       </c>
       <c r="B9" s="1">
-        <v>63</v>
+        <v>28</v>
       </c>
       <c r="C9" t="s">
         <v>8</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:4" ht="15">
       <c r="A10" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B10" s="1">
-        <v>878</v>
+        <v>678</v>
       </c>
       <c r="C10" t="s">
         <v>9</v>
       </c>
       <c r="D10" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="15">
       <c r="A11" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B11" s="1">
-        <v>146</v>
+        <v>113</v>
       </c>
       <c r="C11" t="s">
         <v>10</v>
       </c>
       <c r="D11" t="s">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="15">
       <c r="A12" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B12" s="1">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="C12" t="s">
         <v>9</v>
       </c>
       <c r="D12" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="15">
       <c r="A13" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B13" s="1">
-        <v>3</v>
+        <v>31</v>
       </c>
       <c r="C13" t="s">
         <v>10</v>
       </c>
       <c r="D13" t="s">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" ht="15">
       <c r="A14" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B14" s="1">
-        <v>52</v>
+        <v>46</v>
       </c>
       <c r="C14" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:3" ht="15">
       <c r="A15" t="s">
+        <v>19</v>
+      </c>
+      <c r="B15" s="1">
+        <v>371</v>
+      </c>
+      <c r="C15" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="15">
+      <c r="A16" t="s">
         <v>20</v>
       </c>
-      <c r="B15" s="1">
-        <v>412</v>
-      </c>
-      <c r="C15" t="s">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>21</v>
-      </c>
       <c r="B16" s="1">
-        <v>299</v>
+        <v>245</v>
       </c>
       <c r="C16" t="s">
         <v>12</v>
       </c>
       <c r="D16" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="15">
       <c r="A17" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B17" s="1">
-        <v>482</v>
+        <v>394</v>
       </c>
       <c r="C17" t="s">
         <v>13</v>
       </c>
       <c r="D17" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15">
       <c r="A18" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B18" s="1">
-        <v>118</v>
+        <v>87</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
       </c>
       <c r="D18" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15">
       <c r="A19" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B19" s="1">
-        <v>69</v>
+        <v>34</v>
       </c>
       <c r="C19" t="s">
         <v>15</v>
       </c>
       <c r="D19" t="s">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="15">
       <c r="A20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B20" s="1">
-        <v>35</v>
+        <v>27</v>
       </c>
       <c r="C20" t="s">
         <v>12</v>
@@ -748,12 +847,12 @@
         <v>8</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:4" ht="15">
       <c r="A21" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B21" s="1">
-        <v>27</v>
+        <v>14</v>
       </c>
       <c r="C21" t="s">
         <v>13</v>
@@ -762,9 +861,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:4" ht="15">
       <c r="A22" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B22" s="1">
         <v>0</v>
@@ -776,9 +875,9 @@
         <v>8</v>
       </c>
     </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:4" ht="15">
       <c r="A23" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B23" s="1">
         <v>1</v>
@@ -791,8 +890,7 @@
       </c>
     </row>
   </sheetData>
-  <phoneticPr fontId="1" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" paperSize="1" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>